<commit_message>
doc modified & added
</commit_message>
<xml_diff>
--- a/doc/Team SCHEDULE Form.xlsx
+++ b/doc/Team SCHEDULE Form.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -711,10 +711,18 @@
         <f>D18/$D$21</f>
         <v>0.21739130434782608</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="F18" s="8">
+        <v>100</v>
+      </c>
+      <c r="G18" s="8">
+        <v>100</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.21739130434782608</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.21739130434782608</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="8">
@@ -734,10 +742,18 @@
         <f>D19/$D$21</f>
         <v>0.47826086956521741</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="F19" s="8">
+        <v>120</v>
+      </c>
+      <c r="G19" s="8">
+        <v>220</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.26090000000000002</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.47826086956521741</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7">

</xml_diff>